<commit_message>
add document comment support
</commit_message>
<xml_diff>
--- a/Y_样本_example.xlsx
+++ b/Y_样本_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8640"/>
+    <workbookView windowWidth="20385" windowHeight="8640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weapon" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119">
+  <si>
+    <t>武器配置</t>
+  </si>
+  <si>
+    <t>这里可以随便写一些注释</t>
+  </si>
+  <si>
+    <t>you can write what you want to write here</t>
+  </si>
+  <si>
+    <t>这此数据不会被导出</t>
+  </si>
   <si>
     <t>array</t>
   </si>
@@ -226,6 +238,9 @@
     <t>*爆炎剑.巴塔路西斯&amp;爆炎师.巴塔路西斯&amp;爆炎拳.巴塔路西斯 掉落(地下城: 远古墓穴深处)*在NPC克伦特的物品店购买(阿拉德陨石 ×150)</t>
   </si>
   <si>
+    <t>英雄配置</t>
+  </si>
+  <si>
     <t>英雄id</t>
   </si>
   <si>
@@ -302,6 +317,9 @@
   </si>
   <si>
     <t>{"测试数据",99,{res = 1,id = 10001,count = 1}}</t>
+  </si>
+  <si>
+    <t>活动配置</t>
   </si>
   <si>
     <t>object</t>
@@ -364,14 +382,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -385,30 +409,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,8 +429,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -443,11 +459,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -460,16 +475,31 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -484,22 +514,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,22 +550,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,25 +572,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,19 +674,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,133 +752,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,17 +781,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -775,11 +799,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -799,13 +829,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -825,17 +859,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -844,152 +874,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -999,8 +1029,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1316,196 +1348,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="4" max="4" width="23.625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" customFormat="1"/>
+    <row r="3" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:6">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="1" ht="13.5" customHeight="1" spans="2:6">
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:6">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="4" s="4" customFormat="1" ht="13.5" customHeight="1" spans="2:6">
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="1" ht="13.5" customHeight="1" spans="2:6">
-      <c r="B5">
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" ht="13.5" customHeight="1" spans="2:6">
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" ht="13.5" customHeight="1" spans="2:6">
-      <c r="B6">
-        <v>1001</v>
-      </c>
-      <c r="C6">
-        <v>85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5" customHeight="1" spans="2:6">
-      <c r="B7">
-        <v>1002</v>
-      </c>
-      <c r="C7">
-        <v>85</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" ht="13.5" customHeight="1" spans="2:6">
       <c r="B8">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C8">
         <v>85</v>
       </c>
       <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" spans="2:6">
       <c r="B9">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" spans="2:6">
       <c r="B10">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C10">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" spans="2:6">
       <c r="B11">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C11">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1514,10 +1534,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1" spans="2:6">
       <c r="B12">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C12">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -1528,85 +1548,85 @@
     </row>
     <row r="13" ht="13.5" customHeight="1" spans="2:6">
       <c r="B13">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C13">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" spans="2:6">
       <c r="B14">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" spans="2:6">
       <c r="B15">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C15">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" ht="13.5" customHeight="1" spans="2:6">
       <c r="B16">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C16">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" spans="2:6">
       <c r="B17">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C17">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" ht="13.5" customHeight="1" spans="2:6">
       <c r="B18">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C18">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" ht="13.5" customHeight="1" spans="2:6">
       <c r="B19">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C19">
         <v>85</v>
@@ -1620,7 +1640,7 @@
     </row>
     <row r="20" ht="13.5" customHeight="1" spans="2:6">
       <c r="B20">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C20">
         <v>85</v>
@@ -1634,7 +1654,7 @@
     </row>
     <row r="21" ht="13.5" customHeight="1" spans="2:6">
       <c r="B21">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C21">
         <v>85</v>
@@ -1648,7 +1668,7 @@
     </row>
     <row r="22" ht="13.5" customHeight="1" spans="2:6">
       <c r="B22">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C22">
         <v>85</v>
@@ -1662,7 +1682,7 @@
     </row>
     <row r="23" ht="13.5" customHeight="1" spans="2:6">
       <c r="B23">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C23">
         <v>85</v>
@@ -1671,40 +1691,40 @@
         <v>51</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" spans="2:6">
       <c r="B24">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="C24">
         <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" spans="2:6">
       <c r="B25">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C25">
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" spans="2:6">
       <c r="B26">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="C26">
         <v>85</v>
@@ -1718,52 +1738,52 @@
     </row>
     <row r="27" ht="13.5" customHeight="1" spans="2:6">
       <c r="B27">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C27">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
         <v>58</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" spans="2:6">
       <c r="B28">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="C28">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" spans="2:6">
       <c r="B29">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C29">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" spans="2:6">
       <c r="B30">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="C30">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -1774,10 +1794,10 @@
     </row>
     <row r="31" ht="13.5" customHeight="1" spans="2:6">
       <c r="B31">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
         <v>65</v>
@@ -1788,16 +1808,44 @@
     </row>
     <row r="32" ht="13.5" customHeight="1" spans="2:6">
       <c r="B32">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="C32">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
         <v>67</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="33" ht="13.5" customHeight="1" spans="2:6">
+      <c r="B33">
+        <v>1026</v>
+      </c>
+      <c r="C33">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" spans="2:6">
+      <c r="B34">
+        <v>1027</v>
+      </c>
+      <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1810,10 +1858,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -1823,172 +1871,178 @@
     <col min="7" max="7" width="52.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:7">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="4" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="4" t="s">
+    </row>
+    <row r="2" customFormat="1"/>
+    <row r="3" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="1" ht="13.5" customHeight="1" spans="2:7">
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" s="4" customFormat="1" ht="13.5" customHeight="1" spans="2:7">
+      <c r="B4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:7">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" ht="13.5" customHeight="1" spans="2:7">
-      <c r="B5">
-        <v>1001</v>
-      </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:7">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" ht="13.5" customHeight="1" spans="2:7">
-      <c r="B6">
-        <v>1002</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" spans="2:7">
       <c r="B7">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="G7" t="s">
         <v>87</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" spans="2:7">
       <c r="B8">
+        <v>1002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" ht="13.5" customHeight="1" spans="2:7">
+      <c r="B9">
+        <v>1003</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" ht="13.5" customHeight="1" spans="2:7">
+      <c r="B10">
         <v>1004</v>
       </c>
-      <c r="C8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" spans="4:4">
-      <c r="D9" t="s">
-        <v>94</v>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" spans="4:4">
+      <c r="D11" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2001,78 +2055,53 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="4" width="9" style="4"/>
     <col min="5" max="5" width="76.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:4">
-      <c r="A1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" ht="13.5" customHeight="1" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1" spans="1:5">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+    </row>
+    <row r="2" customFormat="1"/>
+    <row r="3" s="4" customFormat="1" ht="13.5" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
+        <v>101</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>102</v>
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" spans="1:5">
@@ -2080,16 +2109,16 @@
         <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" t="s">
         <v>105</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" spans="1:5">
@@ -2097,7 +2126,7 @@
         <v>106</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>107</v>
@@ -2105,8 +2134,42 @@
       <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" customHeight="1" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" ht="13.5" customHeight="1" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2184,7 @@
   <sheetPr/>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2137,10 +2200,10 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:3">
@@ -2148,10 +2211,10 @@
         <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" spans="1:3">
@@ -2159,10 +2222,10 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" spans="1:5">
@@ -2170,13 +2233,13 @@
         <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" spans="1:5">
@@ -2184,10 +2247,10 @@
         <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -2196,10 +2259,10 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -2208,10 +2271,10 @@
         <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -2220,7 +2283,7 @@
         <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -2229,13 +2292,13 @@
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" spans="1:5">
@@ -2243,7 +2306,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -2252,7 +2315,7 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -2261,13 +2324,13 @@
         <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" spans="1:3">
@@ -2275,10 +2338,10 @@
         <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" spans="1:3">
@@ -2286,10 +2349,10 @@
         <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" spans="1:3">
@@ -2297,10 +2360,10 @@
         <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" spans="1:3">
@@ -2308,10 +2371,10 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" spans="1:3">
@@ -2319,10 +2382,10 @@
         <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" spans="1:3">
@@ -2330,10 +2393,10 @@
         <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" spans="1:3">
@@ -2341,10 +2404,10 @@
         <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" spans="1:3">
@@ -2352,10 +2415,10 @@
         <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" spans="1:3">
@@ -2363,10 +2426,10 @@
         <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" spans="1:3">
@@ -2374,10 +2437,10 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" spans="1:3">
@@ -2385,10 +2448,10 @@
         <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" spans="1:3">
@@ -2396,10 +2459,10 @@
         <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" spans="1:3">
@@ -2407,10 +2470,10 @@
         <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" spans="1:3">
@@ -2418,10 +2481,10 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" spans="1:3">
@@ -2429,10 +2492,10 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>